<commit_message>
some changes with parser work
</commit_message>
<xml_diff>
--- a/duplicate.xlsx
+++ b/duplicate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="59">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -103,49 +103,91 @@
     <t>data_origin</t>
   </si>
   <si>
-    <t>https://elibrary.ru/item.asp?id=42536552</t>
+    <t>https://elibrary.ru/item.asp?id=41645549</t>
+  </si>
+  <si>
+    <t>https://elibrary.ru/item.asp?id=41645857</t>
+  </si>
+  <si>
+    <t>https://elibrary.ru/item.asp?id=42377157</t>
   </si>
   <si>
     <t>статья в журнале</t>
   </si>
   <si>
+    <t>материалы конференции</t>
+  </si>
+  <si>
     <t>научная статья</t>
   </si>
   <si>
-    <t>Бурение и нефть</t>
-  </si>
-  <si>
-    <t>gsgksgks</t>
-  </si>
-  <si>
-    <t>2072-4799</t>
-  </si>
-  <si>
-    <t>ООО "Бурнефть"</t>
+    <t>Lecture Notes in Etetete</t>
+  </si>
+  <si>
+    <t>Lecture Notes in Electrical Engineering</t>
+  </si>
+  <si>
+    <t>Lecture fsfsfsfs</t>
+  </si>
+  <si>
+    <t>Нефтепромысловое делоshhshsh</t>
+  </si>
+  <si>
+    <t>Нефтепромысловое дело</t>
+  </si>
+  <si>
+    <t>1876-1100</t>
+  </si>
+  <si>
+    <t>0207-2351</t>
+  </si>
+  <si>
+    <t>1876-1119</t>
+  </si>
+  <si>
+    <t>Российский государственный университет нефти и газа (национальный исследовательский университет) им. И.М. Губкина</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
   <si>
     <t>yes</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>55</t>
+    <t>EN</t>
   </si>
   <si>
     <t>RU</t>
   </si>
   <si>
-    <t>To question of safety of offshore oil and gas constructions in Arctic</t>
-  </si>
-  <si>
-    <t>CWMUUU</t>
+    <t>Geometrical computational method to locate hypocenter by signal readings from a three receivers</t>
+  </si>
+  <si>
+    <t>An investigation on signal comparison by measuring of numerical strings similarity</t>
+  </si>
+  <si>
+    <t>Тестирование полимерно-гелевых систем "Темпоскрин-Плюс ВПП" и "Темпоскрин-Люкс" в условиях применения высокоминерализованных агентов закачки при высоких температурах пласта</t>
+  </si>
+  <si>
+    <t>10.1007/978-3-030-14907-9_16</t>
+  </si>
+  <si>
+    <t>10.1007/978-3-030-14907-9_19</t>
+  </si>
+  <si>
+    <t>10.30713/0207-2351-2020-2(614)-32-37</t>
+  </si>
+  <si>
+    <t>YMFJKJ</t>
+  </si>
+  <si>
+    <t>WOVYTY</t>
+  </si>
+  <si>
+    <t>UBTMHM</t>
+  </si>
+  <si>
+    <t>excel</t>
   </si>
   <si>
     <t>sql</t>
@@ -519,7 +561,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AD7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -616,156 +658,480 @@
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="1">
-        <v>487</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>727</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>42536552</v>
+        <v>41645549</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" t="s">
-        <v>35</v>
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>42</v>
       </c>
       <c r="K2" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="M2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="N2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="P2">
         <v>2020</v>
       </c>
-      <c r="Q2" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" t="s">
-        <v>39</v>
-      </c>
-      <c r="U2" t="s">
-        <v>40</v>
+      <c r="S2">
+        <v>554</v>
+      </c>
+      <c r="T2">
+        <v>154</v>
+      </c>
+      <c r="U2">
+        <v>161</v>
       </c>
       <c r="V2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="W2" t="s">
-        <v>42</v>
+        <v>48</v>
+      </c>
+      <c r="X2" t="s">
+        <v>51</v>
       </c>
       <c r="Y2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="Z2">
-        <v>520000</v>
+        <v>373100</v>
       </c>
       <c r="AA2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="AB2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="AC2">
-        <v>2678</v>
+        <v>2</v>
       </c>
       <c r="AD2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:30">
       <c r="A3" s="1">
-        <v>560</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>1107</v>
+        <v>29</v>
       </c>
       <c r="C3">
-        <v>42536552</v>
+        <v>41645549</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" t="s">
-        <v>35</v>
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
+        <v>42</v>
       </c>
       <c r="K3" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="M3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="N3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="P3">
         <v>2020</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3">
+        <v>554</v>
+      </c>
+      <c r="T3">
+        <v>154</v>
+      </c>
+      <c r="U3">
+        <v>161</v>
+      </c>
+      <c r="V3" t="s">
+        <v>46</v>
+      </c>
+      <c r="W3" t="s">
+        <v>48</v>
+      </c>
+      <c r="X3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z3">
+        <v>373100</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC3">
+        <v>2</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>41645857</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4">
+        <v>2020</v>
+      </c>
+      <c r="S4">
+        <v>554</v>
+      </c>
+      <c r="T4">
+        <v>185</v>
+      </c>
+      <c r="U4">
+        <v>194</v>
+      </c>
+      <c r="V4" t="s">
+        <v>46</v>
+      </c>
+      <c r="W4" t="s">
+        <v>49</v>
+      </c>
+      <c r="X4" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z4">
+        <v>290000</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC4">
+        <v>6</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30">
+      <c r="A5" s="1">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>414</v>
+      </c>
+      <c r="C5">
+        <v>41645857</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5">
+        <v>2020</v>
+      </c>
+      <c r="S5">
+        <v>554</v>
+      </c>
+      <c r="T5">
+        <v>185</v>
+      </c>
+      <c r="U5">
+        <v>194</v>
+      </c>
+      <c r="V5" t="s">
+        <v>46</v>
+      </c>
+      <c r="W5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X5" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z5">
+        <v>290000</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC5">
+        <v>6</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>42377157</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
         <v>38</v>
       </c>
-      <c r="T3" t="s">
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" t="s">
+        <v>44</v>
+      </c>
+      <c r="P6">
+        <v>2020</v>
+      </c>
+      <c r="Q6">
+        <v>2</v>
+      </c>
+      <c r="R6">
+        <v>614</v>
+      </c>
+      <c r="T6">
+        <v>32</v>
+      </c>
+      <c r="U6">
+        <v>37</v>
+      </c>
+      <c r="V6" t="s">
+        <v>47</v>
+      </c>
+      <c r="W6" t="s">
+        <v>50</v>
+      </c>
+      <c r="X6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z6">
+        <v>524700</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC6">
+        <v>22</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>377</v>
+      </c>
+      <c r="C7">
+        <v>42377157</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s">
         <v>39</v>
       </c>
-      <c r="U3" t="s">
-        <v>40</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="H7" t="s">
         <v>41</v>
       </c>
-      <c r="W3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y3" t="s">
+      <c r="J7" t="s">
         <v>43</v>
       </c>
-      <c r="Z3">
-        <v>520000</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB3" t="s">
+      <c r="K7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M7" t="s">
+        <v>44</v>
+      </c>
+      <c r="N7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P7">
+        <v>2020</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>614</v>
+      </c>
+      <c r="T7">
+        <v>32</v>
+      </c>
+      <c r="U7">
         <v>37</v>
       </c>
-      <c r="AC3">
-        <v>2678</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>44</v>
+      <c r="V7" t="s">
+        <v>47</v>
+      </c>
+      <c r="W7" t="s">
+        <v>50</v>
+      </c>
+      <c r="X7" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z7">
+        <v>524700</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC7">
+        <v>22</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>